<commit_message>
add more annotated images and remove old files
</commit_message>
<xml_diff>
--- a/eyelink_data/aois.xlsx
+++ b/eyelink_data/aois.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\simontitk\projects\python\gaze3p\eyelink_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D1677-C02D-43C5-950D-982D413BBB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AB5596-F8D8-423F-829D-D5C70F5BC0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
   <si>
     <t>img</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>2017_98830509.jpg</t>
+  </si>
+  <si>
+    <t>2017_86643084.jpg</t>
+  </si>
+  <si>
+    <t>2017_75065350.jpg</t>
+  </si>
+  <si>
+    <t>2017_20109260.jpg</t>
+  </si>
+  <si>
+    <t>2017_21201684.jpg</t>
+  </si>
+  <si>
+    <t>2017_41698707.jpg</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -121,11 +136,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -143,6 +167,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -450,10 +486,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,6 +1100,258 @@
         <v>250</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0</v>
+      </c>
+      <c r="C44" s="6">
+        <v>150</v>
+      </c>
+      <c r="D44" s="6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8">
+        <v>600</v>
+      </c>
+      <c r="D45" s="8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="10">
+        <v>2</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1150</v>
+      </c>
+      <c r="D46" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="6">
+        <v>0</v>
+      </c>
+      <c r="C47" s="6">
+        <v>400</v>
+      </c>
+      <c r="D47" s="6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6">
+        <v>450</v>
+      </c>
+      <c r="D48" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="6">
+        <v>2</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D49" s="6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="10">
+        <v>3</v>
+      </c>
+      <c r="C50" s="10">
+        <v>650</v>
+      </c>
+      <c r="D50" s="10">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="6">
+        <v>0</v>
+      </c>
+      <c r="C51" s="6">
+        <v>300</v>
+      </c>
+      <c r="D51" s="6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="6">
+        <v>500</v>
+      </c>
+      <c r="D52" s="6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="6">
+        <v>2</v>
+      </c>
+      <c r="C53" s="6">
+        <v>650</v>
+      </c>
+      <c r="D53" s="6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="10">
+        <v>3</v>
+      </c>
+      <c r="C54" s="10">
+        <v>900</v>
+      </c>
+      <c r="D54" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="6">
+        <v>0</v>
+      </c>
+      <c r="C55" s="6">
+        <v>200</v>
+      </c>
+      <c r="D55" s="6">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="6">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6">
+        <v>450</v>
+      </c>
+      <c r="D56" s="6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="6">
+        <v>2</v>
+      </c>
+      <c r="C57" s="6">
+        <v>700</v>
+      </c>
+      <c r="D57" s="6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="10">
+        <v>3</v>
+      </c>
+      <c r="C58" s="10">
+        <v>850</v>
+      </c>
+      <c r="D58" s="10">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="6">
+        <v>0</v>
+      </c>
+      <c r="C59" s="6">
+        <v>180</v>
+      </c>
+      <c r="D59" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="6">
+        <v>1</v>
+      </c>
+      <c r="C60" s="6">
+        <v>700</v>
+      </c>
+      <c r="D60" s="6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="10">
+        <v>2</v>
+      </c>
+      <c r="C61" s="10">
+        <v>1150</v>
+      </c>
+      <c r="D61" s="10">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>